<commit_message>
fix: Rerun the pipeline process
</commit_message>
<xml_diff>
--- a/metadata/lcms/todo/Vanderbilt TMC (LC-MS).xlsx
+++ b/metadata/lcms/todo/Vanderbilt TMC (LC-MS).xlsx
@@ -13,7 +13,7 @@
     <sheet name="Invalid Input Pattern" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Missing Required Value'!$A$1:$D$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Invalid Input Pattern'!$A$1:$F$52</definedName>
   </definedNames>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,25 +431,20 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SCN400</t>
+          <t>cIMS</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>cIMS</t>
+          <t>hour</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>hour</t>
+          <t>microPOTS</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>microPOTS</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>Profiling</t>
         </is>
@@ -458,25 +453,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>STELLARIS 5</t>
+          <t>TWIMS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TWIMS</t>
+          <t>month</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>nanoSPLITS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>nanoSPLITS</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
         <is>
           <t>Imaging</t>
         </is>
@@ -485,20 +475,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BZ-X710</t>
+          <t>DTIMS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DTIMS</t>
+          <t>year</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>year</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>LESA</t>
         </is>
@@ -507,20 +492,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pannoramic MIDI II Digital Scanner</t>
+          <t>SLIM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SLIM</t>
+          <t>day</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>microLESA</t>
         </is>
@@ -529,20 +509,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Not applicable</t>
+          <t>TIMS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TIMS</t>
+          <t>minute</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>minute</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t>nanoPOTS</t>
         </is>
@@ -551,514 +526,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MoticEasyScan One</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
           <t>FAIMS</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>LCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>EVOS M7000</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NovaSeq X</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>NanoZoomer 2.0-HT</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>timsTOF Ultra 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Lightsheet 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Phenocycler-Fusion 1.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>DNBSEQ-T7</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>timsTOF Pro</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>AVITI</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>timsTOF Pro 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Q Exactive UHMR</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Q Exactive</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>timsTOF SCP</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Zyla 4.2 sCMOS</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Helios</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>uScopeHXII-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Custom: Multiphoton</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>QTRAP 5500</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>timsTOF Ultra</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>BZ-X800</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CyTOF 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>G4X Spatial Sequencer</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>NextSeq 500</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>NanoZoomer S360</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Hyperion Imaging System</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>NovaSeq X Plus</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CyTOF XT</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>NanoZoomer-SQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>NextSeq 550</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Axio Zoom.V16</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Digital Spatial Profiler</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>timsTOF FleX</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>timsTOF FleX MALDI-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>NanoZoomer S210</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>BZ-X810</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Axio Observer 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Cytek Northern Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>IN Cell Analyzer 2200</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>timsTOF HT</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>PhenoImager Fusion</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>DM6 B</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Phenocycler-Fusion 2.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Aperio CS2</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Lumos Tribrid</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Resolve Biosciences Molecular Cartography</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>MALDI timsTOF Flex Prototype</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>TissueScope LE Slide Scanner</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>VS200 Slide Scanner</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Axio Observer 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Axio Observer 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>HiSeq 2500</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Orbitrap Eclipse Tribrid</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Cell DIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>MERSCOPE</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>NextSeq 2000</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>NovaSeq 6000</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>In-House</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>HiSeq 4000</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>solariX</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Panoramic 150 Digital Scanner</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Aperio AT2</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>MIBIscope</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Biomark HD</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>NanoZoomer S60</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>CosMx Spatial Molecular Imager</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>MERSCOPE Ultra</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Axio Scan.Z1</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Juno System</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Q Exactive HF</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Xenium Analyzer</t>
         </is>
       </c>
     </row>
@@ -1073,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,23 +584,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HBM234.FFHQ.425</t>
+          <t>HBM235.KWRX.762</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>ion_mobility</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM234.FFHQ.425</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM235.KWRX.762</t>
         </is>
       </c>
     </row>
@@ -1139,7 +608,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -1158,7 +627,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -1172,19 +641,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HBM235.KWRX.762</t>
+          <t>HBM237.TZFG.599</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM235.KWRX.762</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM237.TZFG.599</t>
         </is>
       </c>
     </row>
@@ -1196,7 +665,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1215,7 +684,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -1229,72 +698,64 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HBM237.TZFG.599</t>
+          <t>HBM278.QSHT.258</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM237.TZFG.599</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HBM264.LNQW.373</t>
+          <t>HBM278.QSHT.258</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_technique</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM264.LNQW.373</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HBM276.ZMTV.784</t>
+          <t>HBM278.QSHT.258</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_type</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM276.ZMTV.784</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HBM278.QSHT.258</t>
+          <t>HBM462.PQHM.967</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1306,14 +767,14 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HBM278.QSHT.258</t>
+          <t>HBM462.PQHM.967</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1325,14 +786,14 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HBM278.QSHT.258</t>
+          <t>HBM462.PQHM.967</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1344,266 +805,242 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM278.QSHT.258</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HBM344.HKXT.423</t>
+          <t>HBM476.FLFT.375</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>ion_mobility</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM344.HKXT.423</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HBM348.TLKL.662</t>
+          <t>HBM476.FLFT.375</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_technique</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM348.TLKL.662</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HBM355.VDXT.245</t>
+          <t>HBM476.FLFT.375</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_type</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM355.VDXT.245</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HBM435.MKRV.485</t>
+          <t>HBM584.XGQT.447</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>ion_mobility</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM435.MKRV.485</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HBM449.SKWJ.362</t>
+          <t>HBM584.XGQT.447</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_technique</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM449.SKWJ.362</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HBM462.PQHM.967</t>
+          <t>HBM584.XGQT.447</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HBM462.PQHM.967</t>
+          <t>HBM668.QZWH.548</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HBM462.PQHM.967</t>
+          <t>HBM668.QZWH.548</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM462.PQHM.967</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>HBM476.FLFT.375</t>
+          <t>HBM668.QZWH.548</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HBM476.FLFT.375</t>
+          <t>HBM689.LCZJ.635</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HBM476.FLFT.375</t>
+          <t>HBM689.LCZJ.635</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM476.FLFT.375</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>HBM569.KMPP.778</t>
+          <t>HBM689.LCZJ.635</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_type</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM569.KMPP.778</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HBM584.XGQT.447</t>
+          <t>HBM727.FSLG.823</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1615,14 +1052,14 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HBM584.XGQT.447</t>
+          <t>HBM727.FSLG.823</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1634,14 +1071,14 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HBM584.XGQT.447</t>
+          <t>HBM727.FSLG.823</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1653,197 +1090,185 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM584.XGQT.447</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>HBM668.JLFW.397</t>
+          <t>HBM754.SZQQ.629</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>ion_mobility</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM668.JLFW.397</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HBM668.QZWH.548</t>
+          <t>HBM754.SZQQ.629</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HBM668.QZWH.548</t>
+          <t>HBM754.SZQQ.629</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>HBM668.QZWH.548</t>
+          <t>HBM765.XFHR.246</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM668.QZWH.548</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HBM689.LCZJ.635</t>
+          <t>HBM765.XFHR.246</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>HBM689.LCZJ.635</t>
+          <t>HBM765.XFHR.246</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>HBM689.LCZJ.635</t>
+          <t>HBM776.ZDWT.399</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM689.LCZJ.635</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>HBM695.BJZM.557</t>
+          <t>HBM776.ZDWT.399</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_technique</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM695.BJZM.557</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HBM726.VXBQ.393</t>
+          <t>HBM776.ZDWT.399</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>spatial_sampling_type</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM726.VXBQ.393</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>HBM727.FSLG.823</t>
+          <t>HBM848.ZBMT.962</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1855,14 +1280,14 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>HBM727.FSLG.823</t>
+          <t>HBM848.ZBMT.962</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1874,14 +1299,14 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>HBM727.FSLG.823</t>
+          <t>HBM848.ZBMT.962</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1893,504 +1318,135 @@
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM727.FSLG.823</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>HBM748.GPDM.692</t>
+          <t>HBM863.ZHZF.274</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
+          <t>ion_mobility</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM748.GPDM.692</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>HBM754.SZQQ.629</t>
+          <t>HBM863.ZHZF.274</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>HBM754.SZQQ.629</t>
+          <t>HBM863.ZHZF.274</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>HBM754.SZQQ.629</t>
+          <t>HBM935.LPGG.796</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>spatial_sampling_type</t>
+          <t>ion_mobility</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM754.SZQQ.629</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM935.LPGG.796</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>HBM765.XFHR.246</t>
+          <t>HBM935.LPGG.796</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ion_mobility</t>
+          <t>spatial_sampling_technique</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
+          <t>https://portal.hubmapconsortium.org/browse/HBM935.LPGG.796</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>HBM765.XFHR.246</t>
+          <t>HBM935.LPGG.796</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>spatial_sampling_technique</t>
+          <t>spatial_sampling_type</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>HBM765.XFHR.246</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>spatial_sampling_type</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM765.XFHR.246</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>HBM776.ZDWT.399</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>ion_mobility</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>HBM776.ZDWT.399</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>spatial_sampling_technique</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>HBM776.ZDWT.399</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>spatial_sampling_type</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM776.ZDWT.399</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>HBM787.FMCW.347</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM787.FMCW.347</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>HBM793.KFWG.238</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM793.KFWG.238</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>HBM829.WPMT.279</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM829.WPMT.279</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>HBM848.ZBMT.962</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>ion_mobility</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>HBM848.ZBMT.962</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>spatial_sampling_technique</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>HBM848.ZBMT.962</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>spatial_sampling_type</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM848.ZBMT.962</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>HBM863.ZHZF.274</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>ion_mobility</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>HBM863.ZHZF.274</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>spatial_sampling_technique</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>HBM863.ZHZF.274</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>spatial_sampling_type</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM863.ZHZF.274</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>HBM935.LPGG.796</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>ion_mobility</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr">
-        <is>
           <t>https://portal.hubmapconsortium.org/browse/HBM935.LPGG.796</t>
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>HBM935.LPGG.796</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>spatial_sampling_technique</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM935.LPGG.796</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>HBM935.LPGG.796</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>spatial_sampling_type</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM935.LPGG.796</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>HBM938.FRHG.524</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM938.FRHG.524</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>HBM952.RNFS.983</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>acquisition_instrument_model</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Orbitrap Fusion Tribrid</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM952.RNFS.983</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E64"/>
-  <dataValidations count="4">
-    <dataValidation sqref="D2 D9 D10 D14 D15 D16 D17 D18 D25 D29 D36 D37 D41 D51 D52 D53 D63 D64" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$A$1:$A$77</formula1>
+  <autoFilter ref="A1:E46"/>
+  <dataValidations count="3">
+    <dataValidation sqref="D2 D5 D8 D11 D14 D17 D20 D23 D26 D29 D32 D35 D38 D41 D44" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$A$1:$A$6</formula1>
     </dataValidation>
-    <dataValidation sqref="D3 D6 D11 D19 D22 D26 D30 D33 D38 D42 D45 D48 D54 D57 D60" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$B$1:$B$6</formula1>
+    <dataValidation sqref="D3 D6 D9 D12 D15 D18 D21 D24 D27 D30 D33 D36 D39 D42 D45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$C$1:$C$6</formula1>
     </dataValidation>
-    <dataValidation sqref="D4 D7 D12 D20 D23 D27 D31 D34 D39 D43 D46 D49 D55 D58 D61" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$D$1:$D$6</formula1>
-    </dataValidation>
-    <dataValidation sqref="D5 D8 D13 D21 D24 D28 D32 D35 D40 D44 D47 D50 D56 D59 D62" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$E$1:$E$2</formula1>
+    <dataValidation sqref="D4 D7 D10 D13 D16 D19 D22 D25 D28 D31 D34 D37 D40 D43 D46" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$D$1:$D$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3949,7 +3005,7 @@
   <autoFilter ref="A1:D85"/>
   <dataValidations count="1">
     <dataValidation sqref="C3 C5 C7 C10 C13 C15 C18 C21 C24 C27 C30 C32 C34 C37 C39 C42 C44 C46 C49 C52 C54 C57 C59 C61 C63 C66 C69 C72 C74 C76 C78 C81 C84" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$C$1:$C$5</formula1>
+      <formula1>_validation_data!$B$1:$B$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>